<commit_message>
added weekly filter in report page
</commit_message>
<xml_diff>
--- a/src/main/resources/data/Report.xlsx
+++ b/src/main/resources/data/Report.xlsx
@@ -15,7 +15,7 @@
     <sheet name="report-sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'report-sheet'!$A$1:$A$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'report-sheet'!$A$1:$A$10</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Sold (as) X 11</t>
+  </si>
+  <si>
+    <t>Bought (Third Party PD - 1) X 1</t>
   </si>
 </sst>
 </file>
@@ -92,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -381,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,8 +409,8 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>44864.147488425922</v>
+      <c r="A2" s="8">
+        <v>44865.147488425922</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -416,73 +420,106 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="8">
+        <v>44858.147488425922</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>148.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>44857.147488425922</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>148.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>44834.147303240738</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C5">
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>44805.146689814814</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>-150</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>44835.146099537036</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="C7">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>44562.144895833335</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <v>44561.144988425927</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>299</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
         <v>44407.144861111112</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C10">
         <v>24</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>44864.623365555555</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>-12</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:A8"/>
+  <autoFilter ref="A1:A10"/>
   <sortState ref="A2:C8">
     <sortCondition descending="1" ref="A1"/>
   </sortState>

</xml_diff>